<commit_message>
tunings BEALE nos xlsx + execucoes nos xlsx + tuning_q_c_stdmin [WIP]
</commit_message>
<xml_diff>
--- a/ExecucoesGerais/tuning/tuning_perturbacao_original.xlsx
+++ b/ExecucoesGerais/tuning/tuning_perturbacao_original.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14460" windowHeight="7935"/>
+    <workbookView windowWidth="14460" windowHeight="7965" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GRI" sheetId="4" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="ROS" sheetId="1" r:id="rId3"/>
     <sheet name="SCH" sheetId="2" r:id="rId4"/>
     <sheet name="ACK" sheetId="3" r:id="rId5"/>
+    <sheet name="BEA" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="11">
   <si>
     <t>GRIEWANGK - MELHORFX</t>
   </si>
@@ -58,10 +59,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -80,78 +81,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -164,23 +95,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,7 +112,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,12 +128,96 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -233,7 +234,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,7 +282,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,13 +354,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,67 +366,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,55 +384,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,7 +402,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,6 +425,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -445,21 +461,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -467,6 +468,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -481,21 +497,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -529,148 +530,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -678,22 +679,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -759,9 +760,9 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="false"/>
+  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="false"/>
+  <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
@@ -774,7 +775,7 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr defTabSz="914400">
@@ -799,7 +800,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -808,7 +809,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="false"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -823,7 +824,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="false"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -863,7 +864,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -931,7 +932,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -974,7 +975,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -1042,15 +1043,15 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="false"/>
-          <c:showVal val="false"/>
-          <c:showCatName val="false"/>
-          <c:showSerName val="false"/>
-          <c:showPercent val="false"/>
-          <c:showBubbleSize val="false"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:axId val="36553957"/>
         <c:axId val="742628703"/>
@@ -1102,7 +1103,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -1189,7 +1190,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -1238,7 +1239,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -1325,7 +1326,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -1374,7 +1375,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -1461,7 +1462,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -1510,7 +1511,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -1597,7 +1598,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
           </c:ext>
@@ -1610,12 +1611,12 @@
           <c:max val="1.8"/>
           <c:min val="0.4"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -1640,7 +1641,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1649,7 +1650,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="false"/>
+        <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -1664,7 +1665,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1691,12 +1692,12 @@
           <c:orientation val="minMax"/>
           <c:max val="20000"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -1721,7 +1722,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1730,7 +1731,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="false"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -1745,7 +1746,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1777,7 +1778,7 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1786,7 +1787,7 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
@@ -1805,9 +1806,9 @@
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="true"/>
+    <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="false"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1843,9 +1844,9 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="false"/>
+  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="false"/>
+  <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
@@ -1858,7 +1859,7 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr defTabSz="914400">
@@ -1883,7 +1884,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1892,7 +1893,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="false"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1907,7 +1908,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="false"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -1947,7 +1948,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -2057,7 +2058,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2100,7 +2101,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -2210,15 +2211,15 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="false"/>
-          <c:showVal val="false"/>
-          <c:showCatName val="false"/>
-          <c:showSerName val="false"/>
-          <c:showPercent val="false"/>
-          <c:showBubbleSize val="false"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:axId val="36553957"/>
         <c:axId val="742628703"/>
@@ -2270,7 +2271,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -2357,7 +2358,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -2406,7 +2407,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -2493,7 +2494,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -2542,7 +2543,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -2629,7 +2630,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -2678,7 +2679,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -2765,7 +2766,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
           </c:ext>
@@ -2776,12 +2777,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -2806,7 +2807,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2815,7 +2816,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="false"/>
+        <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -2830,7 +2831,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2857,12 +2858,12 @@
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -2887,7 +2888,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2896,7 +2897,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="false"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -2911,7 +2912,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2941,7 +2942,7 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2950,7 +2951,7 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
@@ -2969,9 +2970,9 @@
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="true"/>
+    <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="false"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2998,16 +2999,16 @@
     </a:p>
   </c:txPr>
   <c:externalData r:id="rId1">
-    <c:autoUpdate val="false"/>
+    <c:autoUpdate val="0"/>
   </c:externalData>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="false"/>
+  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="false"/>
+  <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
@@ -3020,7 +3021,7 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr defTabSz="914400">
@@ -3045,7 +3046,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3054,7 +3055,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="false"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -3069,7 +3070,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="false"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -3108,7 +3109,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -3176,7 +3177,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3219,7 +3220,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -3287,15 +3288,15 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="false"/>
-          <c:showVal val="false"/>
-          <c:showCatName val="false"/>
-          <c:showSerName val="false"/>
-          <c:showPercent val="false"/>
-          <c:showBubbleSize val="false"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:axId val="891020920"/>
         <c:axId val="342195230"/>
@@ -3347,7 +3348,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -3434,7 +3435,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -3483,7 +3484,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -3570,7 +3571,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -3619,7 +3620,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -3706,7 +3707,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -3755,7 +3756,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -3842,7 +3843,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
           </c:ext>
@@ -3855,12 +3856,12 @@
           <c:max val="1.8"/>
           <c:min val="0.4"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -3885,7 +3886,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -3894,7 +3895,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="false"/>
+        <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -3909,7 +3910,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -3935,12 +3936,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -3965,7 +3966,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -3974,7 +3975,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="true"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -3989,7 +3990,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4021,7 +4022,7 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4030,7 +4031,7 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
@@ -4049,9 +4050,9 @@
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="true"/>
+    <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="false"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4087,9 +4088,9 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="false"/>
+  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="false"/>
+  <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
@@ -4102,7 +4103,7 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr defTabSz="914400">
@@ -4127,7 +4128,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4136,7 +4137,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="false"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -4151,7 +4152,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="false"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -4191,7 +4192,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -4301,7 +4302,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -4344,7 +4345,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -4454,15 +4455,15 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="false"/>
-          <c:showVal val="false"/>
-          <c:showCatName val="false"/>
-          <c:showSerName val="false"/>
-          <c:showPercent val="false"/>
-          <c:showBubbleSize val="false"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:axId val="510780898"/>
         <c:axId val="608920304"/>
@@ -4514,7 +4515,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -4703,7 +4704,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -4752,7 +4753,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -4941,7 +4942,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -4990,7 +4991,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -5179,7 +5180,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -5228,7 +5229,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -5417,7 +5418,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
           </c:ext>
@@ -5430,12 +5431,12 @@
           <c:max val="3"/>
           <c:min val="0.2"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -5460,7 +5461,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -5469,7 +5470,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="false"/>
+        <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -5484,7 +5485,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5511,12 +5512,12 @@
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -5541,7 +5542,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -5550,7 +5551,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0E+00" sourceLinked="false"/>
+        <c:numFmt formatCode="0E+00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -5566,7 +5567,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5596,7 +5597,7 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -5605,7 +5606,7 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
@@ -5624,9 +5625,9 @@
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="true"/>
+    <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="false"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5662,9 +5663,9 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="false"/>
+  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="false"/>
+  <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
@@ -5677,7 +5678,7 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr defTabSz="914400">
@@ -5709,7 +5710,7 @@
           <c:y val="0.0252365930599369"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -5718,7 +5719,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="false"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -5733,7 +5734,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="false"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -5772,7 +5773,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -5882,7 +5883,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -5925,7 +5926,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -6035,15 +6036,15 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="false"/>
-          <c:showVal val="false"/>
-          <c:showCatName val="false"/>
-          <c:showSerName val="false"/>
-          <c:showPercent val="false"/>
-          <c:showBubbleSize val="false"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:axId val="431151722"/>
         <c:axId val="49984735"/>
@@ -6095,7 +6096,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -6284,7 +6285,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -6333,7 +6334,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -6522,7 +6523,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -6571,7 +6572,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -6760,7 +6761,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -6809,7 +6810,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -6998,7 +6999,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
           </c:ext>
@@ -7011,12 +7012,12 @@
           <c:max val="3"/>
           <c:min val="0.2"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -7041,7 +7042,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -7050,7 +7051,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="false"/>
+        <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -7065,7 +7066,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -7091,12 +7092,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -7128,7 +7129,7 @@
               <c:y val="0.410589782942337"/>
             </c:manualLayout>
           </c:layout>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -7137,7 +7138,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="false"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -7152,7 +7153,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -7184,7 +7185,7 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -7193,7 +7194,7 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
@@ -7212,9 +7213,9 @@
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="true"/>
+    <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="false"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -7250,9 +7251,9 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="false"/>
+  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="false"/>
+  <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
@@ -7265,7 +7266,7 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr defTabSz="914400">
@@ -7290,7 +7291,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -7299,7 +7300,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="false"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -7314,7 +7315,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="false"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -7354,7 +7355,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -7464,7 +7465,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -7507,7 +7508,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:delete val="true"/>
+            <c:delete val="1"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
@@ -7617,15 +7618,15 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="true"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="false"/>
-          <c:showVal val="false"/>
-          <c:showCatName val="false"/>
-          <c:showSerName val="false"/>
-          <c:showPercent val="false"/>
-          <c:showBubbleSize val="false"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:axId val="823537699"/>
         <c:axId val="944737202"/>
@@ -7677,7 +7678,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -7908,7 +7909,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -7957,7 +7958,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -8188,7 +8189,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -8237,7 +8238,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -8450,7 +8451,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
             <c15:filteredScatterSeries>
@@ -8499,7 +8500,7 @@
                   </c:spPr>
                 </c:marker>
                 <c:dLbls>
-                  <c:delete val="true"/>
+                  <c:delete val="1"/>
                 </c:dLbls>
                 <c:xVal>
                   <c:numRef>
@@ -8730,7 +8731,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
-                <c:smooth val="true"/>
+                <c:smooth val="1"/>
               </c15:ser>
             </c15:filteredScatterSeries>
           </c:ext>
@@ -8743,12 +8744,12 @@
           <c:max val="3"/>
           <c:min val="0.2"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -8773,7 +8774,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -8782,7 +8783,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="true"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -8797,7 +8798,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -8825,12 +8826,12 @@
           <c:orientation val="minMax"/>
           <c:min val="1e-18"/>
         </c:scaling>
-        <c:delete val="false"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr defTabSz="914400">
@@ -8855,7 +8856,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="false"/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -8864,7 +8865,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0E+00" sourceLinked="false"/>
+        <c:numFmt formatCode="0E+00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
@@ -8879,7 +8880,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -8910,7 +8911,7 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
-      <c:overlay val="false"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -8919,7 +8920,7 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="true"/>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
@@ -8938,9 +8939,9 @@
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="true"/>
+    <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="false"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -8971,6 +8972,622 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr defTabSz="914400">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT" altLang="en-US"/>
+              <a:t>BEALE</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.146419180201083"/>
+          <c:y val="0.262544014084507"/>
+          <c:w val="0.821252900232018"/>
+          <c:h val="0.539260563380282"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BEA!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AGEO1real1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>BEA!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>BEA!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4.8013781914385</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.195058207612</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.49854221721199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4659487026215</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.53417924763222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.839786099103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.00972518572394</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0282661106646159</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00979172721630025</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.7255595436629</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>462.155548337262</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1900.66866656179</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3102.54529309559</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>884.268377479465</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3370.75550060869</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BEA!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AGEO2real1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>BEA!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>BEA!$C$2:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4.6729460950081</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.87271985383333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.01909492268207</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.13159721527807</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.39483689823256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.973373213646788</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.423175353326232</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00749589618741299</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00318367649612149</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0958011573384165</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1761.45901638742</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1903.18359714372</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5433.10870045129</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1126.3378737842</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2348.283877612</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="823537699"/>
+        <c:axId val="944737202"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="823537699"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3"/>
+          <c:min val="0.2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr defTabSz="914400">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" altLang="en-US"/>
+                  <a:t>std</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="944737202"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.4"/>
+        <c:minorUnit val="0.2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="944737202"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr defTabSz="914400">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" altLang="en-US"/>
+                  <a:t>melhor f(x)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-PT" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0E+00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="823537699"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-US"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:externalData r:id="rId1">
+    <c:autoUpdate val="0"/>
+  </c:externalData>
 </c:chartSpace>
 </file>
 
@@ -9214,6 +9831,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -9310,7 +9967,7 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="true">
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
@@ -9826,7 +10483,7 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="true">
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
@@ -10342,7 +10999,7 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="true">
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
@@ -10858,7 +11515,7 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="true">
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
@@ -11374,7 +12031,7 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="true">
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
@@ -11890,7 +12547,523 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="true">
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
@@ -12515,6 +13688,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>227330</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>137795</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>484505</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>127635</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="2837180" y="2671445"/>
+        <a:ext cx="4105275" cy="2885440"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -12633,7 +13841,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -12657,9 +13865,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -12683,7 +13891,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -12736,7 +13944,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -12761,7 +13969,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -12775,23 +13983,23 @@
   <sheetPr/>
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N11" workbookViewId="0">
+    <sheetView topLeftCell="N11" workbookViewId="0">
       <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="4.375" customWidth="true"/>
-    <col min="2" max="3" width="12.625" customWidth="true"/>
-    <col min="4" max="4" width="12.125" customWidth="true"/>
-    <col min="5" max="6" width="12.625" customWidth="true"/>
-    <col min="7" max="7" width="12.125" customWidth="true"/>
-    <col min="8" max="8" width="3.5" customWidth="true"/>
-    <col min="9" max="9" width="4.375" customWidth="true"/>
-    <col min="10" max="10" width="9.625" customWidth="true"/>
-    <col min="11" max="12" width="12.125" customWidth="true"/>
-    <col min="13" max="13" width="9.625" customWidth="true"/>
-    <col min="14" max="15" width="12.125" customWidth="true"/>
+    <col min="1" max="1" width="4.375" customWidth="1"/>
+    <col min="2" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="12.125" customWidth="1"/>
+    <col min="5" max="6" width="12.625" customWidth="1"/>
+    <col min="7" max="7" width="12.125" customWidth="1"/>
+    <col min="8" max="8" width="3.5" customWidth="1"/>
+    <col min="9" max="9" width="4.375" customWidth="1"/>
+    <col min="10" max="10" width="9.625" customWidth="1"/>
+    <col min="11" max="12" width="12.125" customWidth="1"/>
+    <col min="13" max="13" width="9.625" customWidth="1"/>
+    <col min="14" max="15" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -13469,14 +14677,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="4.375" customWidth="true"/>
-    <col min="2" max="7" width="12.625" customWidth="true"/>
-    <col min="8" max="8" width="2.5" customWidth="true"/>
-    <col min="9" max="9" width="4.375" customWidth="true"/>
-    <col min="10" max="10" width="9.625" customWidth="true"/>
-    <col min="11" max="12" width="12.125" customWidth="true"/>
-    <col min="13" max="13" width="9.625" customWidth="true"/>
-    <col min="14" max="15" width="12.125" customWidth="true"/>
+    <col min="1" max="1" width="4.375" customWidth="1"/>
+    <col min="2" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="2.5" customWidth="1"/>
+    <col min="9" max="9" width="4.375" customWidth="1"/>
+    <col min="10" max="10" width="9.625" customWidth="1"/>
+    <col min="11" max="12" width="12.125" customWidth="1"/>
+    <col min="13" max="13" width="9.625" customWidth="1"/>
+    <col min="14" max="15" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -14088,14 +15296,14 @@
   <sheetPr/>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="G11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
     <col min="2" max="7" width="12.625"/>
-    <col min="8" max="8" width="11.625" customWidth="true"/>
+    <col min="8" max="8" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -14485,7 +15693,7 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
     <col min="2" max="7" width="12.625"/>
-    <col min="8" max="8" width="11.625" customWidth="true"/>
+    <col min="8" max="8" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -14874,9 +16082,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="true"/>
-    <col min="2" max="7" width="12.625" customWidth="true"/>
-    <col min="8" max="8" width="11.75" customWidth="true"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -15246,6 +16454,261 @@
       <c r="G16" s="1">
         <v>2.01616501271928e-14</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="11.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0.2</v>
+      </c>
+      <c r="B2">
+        <v>4.8013781914385</v>
+      </c>
+      <c r="C2">
+        <v>4.6729460950081</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>0.4</v>
+      </c>
+      <c r="B3">
+        <v>5.195058207612</v>
+      </c>
+      <c r="C3">
+        <v>4.87271985383333</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>0.6</v>
+      </c>
+      <c r="B4">
+        <v>5.49854221721199</v>
+      </c>
+      <c r="C4">
+        <v>5.01909492268207</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>0.8</v>
+      </c>
+      <c r="B5">
+        <v>4.4659487026215</v>
+      </c>
+      <c r="C5">
+        <v>3.13159721527807</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2.53417924763222</v>
+      </c>
+      <c r="C6">
+        <v>1.39483689823256</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>1.2</v>
+      </c>
+      <c r="B7">
+        <v>1.839786099103</v>
+      </c>
+      <c r="C7">
+        <v>0.973373213646788</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>1.4</v>
+      </c>
+      <c r="B8">
+        <v>1.00972518572394</v>
+      </c>
+      <c r="C8">
+        <v>0.423175353326232</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>1.6</v>
+      </c>
+      <c r="B9">
+        <v>0.0282661106646159</v>
+      </c>
+      <c r="C9">
+        <v>0.00749589618741299</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>1.8</v>
+      </c>
+      <c r="B10">
+        <v>0.00979172721630025</v>
+      </c>
+      <c r="C10">
+        <v>0.00318367649612149</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>19.7255595436629</v>
+      </c>
+      <c r="C11">
+        <v>0.0958011573384165</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>2.2</v>
+      </c>
+      <c r="B12">
+        <v>462.155548337262</v>
+      </c>
+      <c r="C12">
+        <v>1761.45901638742</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>2.4</v>
+      </c>
+      <c r="B13">
+        <v>1900.66866656179</v>
+      </c>
+      <c r="C13">
+        <v>1903.18359714372</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>2.6</v>
+      </c>
+      <c r="B14">
+        <v>3102.54529309559</v>
+      </c>
+      <c r="C14">
+        <v>5433.10870045129</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>2.8</v>
+      </c>
+      <c r="B15">
+        <v>884.268377479465</v>
+      </c>
+      <c r="C15">
+        <v>1126.3378737842</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>3370.75550060869</v>
+      </c>
+      <c r="C16">
+        <v>2348.283877612</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16"/>
+      <c r="G16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>